<commit_message>
Added Download And Upload Facility
</commit_message>
<xml_diff>
--- a/website/static/Number-Sheets/output.xlsx
+++ b/website/static/Number-Sheets/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -599,36 +599,6 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>CSAI2021005</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Bhavya Chaudhary</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>50</v>
-      </c>
-      <c r="F6" t="n">
-        <v>40</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>140</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>